<commit_message>
Traductor a movimientos Patron
Se logra crear una matriz con movimientos en steps para el motor
</commit_message>
<xml_diff>
--- a/explicacionPatron.xlsx
+++ b/explicacionPatron.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/alexsq_estudiantec_cr/Documents/Semestre 2-2023/Micros/ProyectoGrua/Proyecto_Grua_Micros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A47F902-A838-409E-8DA4-368A6E1293AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{5A47F902-A838-409E-8DA4-368A6E1293AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{555F0842-4AD0-4D5C-ADD5-17DF29D1F20B}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-9495" windowWidth="21840" windowHeight="13140" xr2:uid="{7C785FB9-824B-4977-AFC1-771E7454B4B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7C785FB9-824B-4977-AFC1-771E7454B4B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Suministro</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>(100, 5, 50)</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>steps</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +243,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -385,11 +397,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -420,9 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -453,41 +459,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F26E9E-8072-4331-BEFA-12D4D1D09BDA}">
-  <dimension ref="B6:W30"/>
+  <dimension ref="B4:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,258 +855,591 @@
     <col min="1" max="25" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="P4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="1" t="s">
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="N5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="31">
+        <f>P5+35</f>
+        <v>35</v>
+      </c>
+      <c r="R5" s="31">
+        <f t="shared" ref="R5:Y5" si="0">Q5+35</f>
+        <v>70</v>
+      </c>
+      <c r="S5" s="31">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="T5" s="31">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="U5" s="31">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="V5" s="31">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="W5" s="31">
+        <f t="shared" si="0"/>
+        <v>245</v>
+      </c>
+      <c r="X5" s="31">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="Y5" s="31">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4">
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="33">
+        <f>ROUND(P5*240/19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="33">
+        <f t="shared" ref="Q6:Y6" si="1">ROUND(Q5*240/19,0)</f>
+        <v>442</v>
+      </c>
+      <c r="R6" s="33">
+        <f t="shared" si="1"/>
+        <v>884</v>
+      </c>
+      <c r="S6" s="33">
+        <f t="shared" si="1"/>
+        <v>1326</v>
+      </c>
+      <c r="T6" s="33">
+        <f t="shared" si="1"/>
+        <v>1768</v>
+      </c>
+      <c r="U6" s="33">
+        <f t="shared" si="1"/>
+        <v>2211</v>
+      </c>
+      <c r="V6" s="33">
+        <f t="shared" si="1"/>
+        <v>2653</v>
+      </c>
+      <c r="W6" s="33">
+        <f t="shared" si="1"/>
+        <v>3095</v>
+      </c>
+      <c r="X6" s="33">
+        <f t="shared" si="1"/>
+        <v>3537</v>
+      </c>
+      <c r="Y6" s="33">
+        <f t="shared" si="1"/>
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="3">
+      <c r="G7" s="1"/>
+      <c r="H7" s="2">
         <v>6</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>7</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>8</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>9</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="N7" s="32">
+        <v>0</v>
+      </c>
+      <c r="O7" s="33">
+        <f>ROUND(N7*240/19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>2</v>
+      </c>
+      <c r="R7" s="38">
+        <v>3</v>
+      </c>
+      <c r="S7" s="38">
+        <v>4</v>
+      </c>
+      <c r="T7" s="39">
+        <v>5</v>
+      </c>
+      <c r="U7" s="37">
+        <v>6</v>
+      </c>
+      <c r="V7" s="38">
+        <v>7</v>
+      </c>
+      <c r="W7" s="38">
+        <v>8</v>
+      </c>
+      <c r="X7" s="38">
+        <v>9</v>
+      </c>
+      <c r="Y7" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
         <f>B7+10</f>
         <v>11</v>
       </c>
-      <c r="C8" s="7">
-        <f t="shared" ref="C8:L8" si="0">C7+10</f>
+      <c r="C8" s="6">
+        <f t="shared" ref="C8:L8" si="2">C7+10</f>
         <v>12</v>
       </c>
-      <c r="D8" s="7">
-        <f t="shared" si="0"/>
+      <c r="D8" s="6">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="E8" s="7">
-        <f t="shared" si="0"/>
+      <c r="E8" s="6">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="F8" s="8">
-        <f t="shared" si="0"/>
+      <c r="F8" s="7">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="6">
-        <f t="shared" si="0"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="5">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I8" s="7">
-        <f t="shared" si="0"/>
+      <c r="I8" s="6">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="J8" s="7">
-        <f t="shared" si="0"/>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="K8" s="7">
-        <f t="shared" si="0"/>
+      <c r="K8" s="6">
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="L8" s="8">
-        <f t="shared" si="0"/>
+      <c r="L8" s="7">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <f t="shared" ref="B9:B11" si="1">B8+10</f>
+      <c r="N8" s="31">
+        <v>35</v>
+      </c>
+      <c r="O8" s="33">
+        <f t="shared" ref="O8:O11" si="3">ROUND(N8*240/19,0)</f>
+        <v>442</v>
+      </c>
+      <c r="P8" s="40">
+        <f>P7+10</f>
+        <v>11</v>
+      </c>
+      <c r="Q8" s="41">
+        <f t="shared" ref="Q8:T11" si="4">Q7+10</f>
+        <v>12</v>
+      </c>
+      <c r="R8" s="41">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="S8" s="41">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="T8" s="42">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="U8" s="40">
+        <f t="shared" ref="U8:Y11" si="5">U7+10</f>
+        <v>16</v>
+      </c>
+      <c r="V8" s="41">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="W8" s="41">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="X8" s="41">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="Y8" s="42">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <f t="shared" ref="B9:B11" si="6">B8+10</f>
         <v>21</v>
       </c>
-      <c r="C9" s="7">
-        <f t="shared" ref="C9:C11" si="2">C8+10</f>
+      <c r="C9" s="6">
+        <f t="shared" ref="C9:C11" si="7">C8+10</f>
         <v>22</v>
       </c>
-      <c r="D9" s="7">
-        <f t="shared" ref="D9:D11" si="3">D8+10</f>
+      <c r="D9" s="6">
+        <f t="shared" ref="D9:D11" si="8">D8+10</f>
         <v>23</v>
       </c>
-      <c r="E9" s="7">
-        <f t="shared" ref="E9:E11" si="4">E8+10</f>
+      <c r="E9" s="6">
+        <f t="shared" ref="E9:E11" si="9">E8+10</f>
         <v>24</v>
       </c>
-      <c r="F9" s="8">
-        <f t="shared" ref="F9:F11" si="5">F8+10</f>
+      <c r="F9" s="7">
+        <f t="shared" ref="F9:F11" si="10">F8+10</f>
         <v>25</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="6">
-        <f t="shared" ref="H9:H11" si="6">H8+10</f>
+      <c r="G9" s="1"/>
+      <c r="H9" s="5">
+        <f t="shared" ref="H9:H11" si="11">H8+10</f>
         <v>26</v>
       </c>
-      <c r="I9" s="7">
-        <f t="shared" ref="I9:I11" si="7">I8+10</f>
+      <c r="I9" s="6">
+        <f t="shared" ref="I9:I11" si="12">I8+10</f>
         <v>27</v>
       </c>
-      <c r="J9" s="7">
-        <f t="shared" ref="J9:J11" si="8">J8+10</f>
+      <c r="J9" s="6">
+        <f t="shared" ref="J9:J11" si="13">J8+10</f>
         <v>28</v>
       </c>
-      <c r="K9" s="7">
-        <f t="shared" ref="K9:K11" si="9">K8+10</f>
+      <c r="K9" s="6">
+        <f t="shared" ref="K9:K11" si="14">K8+10</f>
         <v>29</v>
       </c>
-      <c r="L9" s="8">
-        <f t="shared" ref="L9:L11" si="10">L8+10</f>
+      <c r="L9" s="7">
+        <f t="shared" ref="L9:L11" si="15">L8+10</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <f t="shared" si="1"/>
+      <c r="N9" s="32">
+        <f>N8+35</f>
+        <v>70</v>
+      </c>
+      <c r="O9" s="33">
+        <f t="shared" si="3"/>
+        <v>884</v>
+      </c>
+      <c r="P9" s="40">
+        <f t="shared" ref="P9:P11" si="16">P8+10</f>
+        <v>21</v>
+      </c>
+      <c r="Q9" s="41">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="R9" s="41">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="S9" s="41">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="T9" s="42">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="U9" s="40">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="V9" s="41">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="W9" s="41">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="X9" s="41">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="Y9" s="42">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
-      <c r="C10" s="7">
-        <f t="shared" si="2"/>
+      <c r="C10" s="6">
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="9"/>
+        <v>34</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="5">
+        <f t="shared" si="11"/>
+        <v>36</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="12"/>
+        <v>37</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="13"/>
+        <v>38</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="14"/>
+        <v>39</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="N10" s="32">
+        <f t="shared" ref="N10:N11" si="17">N9+35</f>
+        <v>105</v>
+      </c>
+      <c r="O10" s="33">
         <f t="shared" si="3"/>
+        <v>1326</v>
+      </c>
+      <c r="P10" s="40">
+        <f t="shared" si="16"/>
+        <v>31</v>
+      </c>
+      <c r="Q10" s="41">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="R10" s="41">
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
-      <c r="E10" s="7">
+      <c r="S10" s="41">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="F10" s="8">
-        <f t="shared" si="5"/>
+      <c r="T10" s="42">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="6">
+      <c r="U10" s="40">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="V10" s="41">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="W10" s="41">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="X10" s="41">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="Y10" s="42">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8">
         <f t="shared" si="6"/>
-        <v>36</v>
-      </c>
-      <c r="I10" s="7">
+        <v>41</v>
+      </c>
+      <c r="C11" s="9">
         <f t="shared" si="7"/>
-        <v>37</v>
-      </c>
-      <c r="J10" s="7">
+        <v>42</v>
+      </c>
+      <c r="D11" s="9">
         <f t="shared" si="8"/>
-        <v>38</v>
-      </c>
-      <c r="K10" s="7">
+        <v>43</v>
+      </c>
+      <c r="E11" s="9">
         <f t="shared" si="9"/>
-        <v>39</v>
-      </c>
-      <c r="L10" s="8">
+        <v>44</v>
+      </c>
+      <c r="F11" s="10">
         <f t="shared" si="10"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
-        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="8">
+        <f t="shared" si="11"/>
+        <v>46</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="12"/>
+        <v>47</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="13"/>
+        <v>48</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="L11" s="10">
+        <f t="shared" si="15"/>
+        <v>50</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="17"/>
+        <v>140</v>
+      </c>
+      <c r="O11" s="33">
+        <f t="shared" si="3"/>
+        <v>1768</v>
+      </c>
+      <c r="P11" s="43">
+        <f t="shared" si="16"/>
         <v>41</v>
       </c>
-      <c r="C11" s="10">
-        <f t="shared" si="2"/>
+      <c r="Q11" s="44">
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="D11" s="10">
-        <f t="shared" si="3"/>
+      <c r="R11" s="44">
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="E11" s="10">
+      <c r="S11" s="44">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="F11" s="11">
-        <f t="shared" si="5"/>
+      <c r="T11" s="45">
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="9">
-        <f t="shared" si="6"/>
+      <c r="U11" s="43">
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
-      <c r="I11" s="10">
-        <f t="shared" si="7"/>
+      <c r="V11" s="44">
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="J11" s="10">
-        <f t="shared" si="8"/>
+      <c r="W11" s="44">
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="K11" s="10">
-        <f t="shared" si="9"/>
+      <c r="X11" s="44">
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="L11" s="11">
-        <f t="shared" si="10"/>
+      <c r="Y11" s="45">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="N15" s="13">
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N15" s="11">
         <v>100</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="12">
         <v>100</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="12">
         <v>100</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15" s="12">
         <v>100</v>
       </c>
-      <c r="R15" s="15">
+      <c r="R15" s="13">
         <v>100</v>
       </c>
-      <c r="S15" s="24">
+      <c r="S15" s="21">
         <v>100</v>
       </c>
-      <c r="T15" s="25"/>
-      <c r="U15" s="26">
+      <c r="T15" s="22"/>
+      <c r="U15" s="23">
         <v>300</v>
       </c>
-      <c r="V15" s="25"/>
-      <c r="W15" s="27">
+      <c r="V15" s="22"/>
+      <c r="W15" s="24">
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>2</v>
       </c>
@@ -1075,32 +1449,32 @@
       <c r="I16" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N16" s="14">
         <v>200</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="15">
         <v>200</v>
       </c>
-      <c r="P16" s="17">
+      <c r="P16" s="15">
         <v>200</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="15">
         <v>200</v>
       </c>
-      <c r="R16" s="18">
+      <c r="R16" s="16">
         <v>200</v>
       </c>
-      <c r="S16" s="28"/>
-      <c r="T16" s="29">
+      <c r="S16" s="25"/>
+      <c r="T16" s="26">
         <v>100</v>
       </c>
-      <c r="U16" s="29">
+      <c r="U16" s="26">
         <v>300</v>
       </c>
-      <c r="V16" s="29">
+      <c r="V16" s="26">
         <v>200</v>
       </c>
-      <c r="W16" s="30"/>
+      <c r="W16" s="27"/>
     </row>
     <row r="17" spans="3:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
@@ -1112,30 +1486,30 @@
       <c r="I17" t="s">
         <v>35</v>
       </c>
-      <c r="N17" s="16">
+      <c r="N17" s="14">
         <v>300</v>
       </c>
-      <c r="O17" s="17">
+      <c r="O17" s="15">
         <v>300</v>
       </c>
-      <c r="P17" s="17">
+      <c r="P17" s="15">
         <v>300</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="15">
         <v>300</v>
       </c>
-      <c r="R17" s="18">
+      <c r="R17" s="16">
         <v>300</v>
       </c>
-      <c r="S17" s="28">
+      <c r="S17" s="25">
         <v>300</v>
       </c>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29">
+      <c r="T17" s="26"/>
+      <c r="U17" s="26">
         <v>100</v>
       </c>
-      <c r="V17" s="29"/>
-      <c r="W17" s="30">
+      <c r="V17" s="26"/>
+      <c r="W17" s="27">
         <v>200</v>
       </c>
     </row>
@@ -1149,22 +1523,22 @@
       <c r="I18" t="s">
         <v>36</v>
       </c>
-      <c r="N18" s="16"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="29">
+      <c r="N18" s="14"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="26">
         <v>200</v>
       </c>
-      <c r="U18" s="29">
+      <c r="U18" s="26">
         <v>300</v>
       </c>
-      <c r="V18" s="29">
+      <c r="V18" s="26">
         <v>100</v>
       </c>
-      <c r="W18" s="30"/>
+      <c r="W18" s="27"/>
     </row>
     <row r="19" spans="3:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
@@ -1176,20 +1550,20 @@
       <c r="I19" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="31">
+      <c r="N19" s="17"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="28">
         <v>200</v>
       </c>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32">
+      <c r="T19" s="29"/>
+      <c r="U19" s="29">
         <v>300</v>
       </c>
-      <c r="V19" s="32"/>
-      <c r="W19" s="33">
+      <c r="V19" s="29"/>
+      <c r="W19" s="30">
         <v>100</v>
       </c>
     </row>
@@ -1203,16 +1577,16 @@
       <c r="I20" t="s">
         <v>38</v>
       </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
     </row>
     <row r="21" spans="3:23" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
@@ -1224,20 +1598,20 @@
       <c r="I21" t="s">
         <v>39</v>
       </c>
-      <c r="N21" s="23" t="s">
+      <c r="N21" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="34" t="s">
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
     </row>
     <row r="22" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
@@ -1339,11 +1713,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="H6:L6"/>
     <mergeCell ref="N21:R21"/>
     <mergeCell ref="S21:W21"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="U4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se sube la versión con todos los códigos como se van a utilizar con la interfaz
Se sube la versión con todos los códigos como se van a utilizar con la interfaz
</commit_message>
<xml_diff>
--- a/explicacionPatron.xlsx
+++ b/explicacionPatron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/alexsq_estudiantec_cr/Documents/Semestre 2-2023/Micros/ProyectoGrua/Proyecto_Grua_Micros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{5A47F902-A838-409E-8DA4-368A6E1293AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3F71E0E-9B56-4546-9A0A-562CD36EF175}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{5A47F902-A838-409E-8DA4-368A6E1293AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8227CE2-31FA-4200-9FB3-30093B808B76}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7C785FB9-824B-4977-AFC1-771E7454B4B1}"/>
+    <workbookView xWindow="-21720" yWindow="-9495" windowWidth="21840" windowHeight="13140" xr2:uid="{7C785FB9-824B-4977-AFC1-771E7454B4B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -503,15 +503,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -524,6 +515,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,7 +842,7 @@
   <dimension ref="B4:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,20 +851,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34" t="s">
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="N5" s="31" t="s">
@@ -912,35 +912,35 @@
       </c>
     </row>
     <row r="6" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
       <c r="N6" s="31"/>
       <c r="O6" s="33" t="s">
         <v>50</v>
       </c>
       <c r="P6" s="33">
-        <f>ROUND(P5*240/19,0)</f>
+        <f>ROUND(P5*445,0)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="33">
-        <f t="shared" ref="Q6:Y6" si="1">ROUND(Q5*240/19,0)</f>
+        <f>ROUND(Q5*240/19,0)</f>
         <v>442</v>
       </c>
       <c r="R6" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q6:Y6" si="1">ROUND(R5*240/19,0)</f>
         <v>884</v>
       </c>
       <c r="S6" s="33">
@@ -1406,51 +1406,51 @@
       </c>
     </row>
     <row r="12" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N12" s="37">
+      <c r="N12" s="34">
         <f t="shared" si="17"/>
         <v>175</v>
       </c>
-      <c r="O12" s="38">
+      <c r="O12" s="35">
         <f t="shared" ref="O12" si="18">ROUND(N12*240/19,0)</f>
         <v>2211</v>
       </c>
-      <c r="P12" s="39">
+      <c r="P12" s="36">
         <f t="shared" si="16"/>
         <v>51</v>
       </c>
-      <c r="Q12" s="40">
+      <c r="Q12" s="37">
         <f t="shared" si="4"/>
         <v>52</v>
       </c>
-      <c r="R12" s="40">
+      <c r="R12" s="37">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="S12" s="40">
+      <c r="S12" s="37">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="T12" s="41">
+      <c r="T12" s="38">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="U12" s="39">
+      <c r="U12" s="36">
         <f t="shared" si="5"/>
         <v>56</v>
       </c>
-      <c r="V12" s="40">
+      <c r="V12" s="37">
         <f t="shared" si="5"/>
         <v>57</v>
       </c>
-      <c r="W12" s="40">
+      <c r="W12" s="37">
         <f t="shared" si="5"/>
         <v>58</v>
       </c>
-      <c r="X12" s="40">
+      <c r="X12" s="37">
         <f t="shared" si="5"/>
         <v>59</v>
       </c>
-      <c r="Y12" s="41">
+      <c r="Y12" s="38">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
@@ -1646,20 +1646,20 @@
       <c r="I21" t="s">
         <v>39</v>
       </c>
-      <c r="N21" s="35" t="s">
+      <c r="N21" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="36" t="s">
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
     </row>
     <row r="22" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C22" t="s">

</xml_diff>